<commit_message>
Added listed control function tests.
</commit_message>
<xml_diff>
--- a/Keysharp.Tests/Code/ControlTests/Control functions.xlsx
+++ b/Keysharp.Tests/Code/ControlTests/Control functions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP6300\Documents\repos\keysharp\bin\debug\net6.0-windows\TEST SCRIPTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP6300\Documents\repos\keysharp\Keysharp.Tests\Code\ControlTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8175CB5-5838-4FBA-B176-061F143A1E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CFBB9B-39CB-48D4-B6F9-4A32F27074CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="121">
   <si>
     <t>Control</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Not working on control in same GUI</t>
-  </si>
-  <si>
     <t>ControlDeleteItem</t>
   </si>
   <si>
@@ -310,9 +307,6 @@
     <t>control_get_enabled.ahk</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>control_focus.ahk</t>
   </si>
   <si>
@@ -352,13 +346,43 @@
     <t>edit_paste.ahk</t>
   </si>
   <si>
-    <t>Fail*</t>
-  </si>
-  <si>
-    <t>Only "Col4" option fails.</t>
-  </si>
-  <si>
     <t>Fails if line is empty.</t>
+  </si>
+  <si>
+    <t>control_exstyle_cb.ahk</t>
+  </si>
+  <si>
+    <t>Not in guitest.ahk yet</t>
+  </si>
+  <si>
+    <t>control_send.ahk</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>control_get_focus.ahk</t>
+  </si>
+  <si>
+    <t>control_get_index.ahk</t>
+  </si>
+  <si>
+    <t>control_get_items.ahk</t>
+  </si>
+  <si>
+    <t>Also tested w/combobox</t>
+  </si>
+  <si>
+    <t>control_move.ahk</t>
+  </si>
+  <si>
+    <t>Some functionality is there.</t>
+  </si>
+  <si>
+    <t>control_set_checked.ahk</t>
+  </si>
+  <si>
+    <t>control_set_enabled.ahk</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1226,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,6 +1296,9 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
       <c r="F3" t="s">
         <v>16</v>
       </c>
@@ -1289,6 +1316,9 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" t="s">
         <v>19</v>
       </c>
@@ -1307,15 +1337,15 @@
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1332,10 +1362,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1352,36 +1382,36 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
@@ -1392,10 +1422,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1407,15 +1437,15 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -1427,15 +1457,15 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -1447,26 +1477,32 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -1478,54 +1514,75 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
         <v>52</v>
       </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -1536,18 +1593,30 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
         <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1559,15 +1628,15 @@
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
         <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -1579,15 +1648,15 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
         <v>59</v>
-      </c>
-      <c r="B22" t="s">
-        <v>60</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1599,118 +1668,160 @@
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
         <v>61</v>
       </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
         <v>63</v>
       </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
         <v>65</v>
       </c>
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
         <v>68</v>
       </c>
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
       <c r="C27" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
       <c r="C29" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
         <v>75</v>
       </c>
-      <c r="B31" t="s">
-        <v>76</v>
-      </c>
       <c r="C31" t="s">
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -1718,10 +1829,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
         <v>77</v>
-      </c>
-      <c r="B32" t="s">
-        <v>78</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -1733,32 +1844,32 @@
         <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" t="s">
         <v>79</v>
       </c>
-      <c r="B33" t="s">
-        <v>80</v>
-      </c>
       <c r="C33" t="s">
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
         <v>81</v>
-      </c>
-      <c r="B34" t="s">
-        <v>82</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -1770,15 +1881,15 @@
         <v>11</v>
       </c>
       <c r="F34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" t="s">
         <v>83</v>
-      </c>
-      <c r="B35" t="s">
-        <v>84</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -1790,15 +1901,15 @@
         <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
         <v>85</v>
-      </c>
-      <c r="B36" t="s">
-        <v>86</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -1810,18 +1921,18 @@
         <v>22</v>
       </c>
       <c r="F36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G36" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
         <v>87</v>
-      </c>
-      <c r="B37" t="s">
-        <v>88</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
@@ -1833,15 +1944,15 @@
         <v>11</v>
       </c>
       <c r="F37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s">
         <v>89</v>
-      </c>
-      <c r="B38" t="s">
-        <v>90</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -1853,15 +1964,15 @@
         <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" t="s">
         <v>91</v>
-      </c>
-      <c r="B39" t="s">
-        <v>92</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
@@ -1873,24 +1984,24 @@
         <v>11</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" t="s">
         <v>93</v>
       </c>
-      <c r="B40" t="s">
-        <v>94</v>
-      </c>
       <c r="C40" t="s">
         <v>9</v>
       </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
       <c r="E40" t="s">
-        <v>110</v>
-      </c>
-      <c r="G40" t="s">
-        <v>111</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>